<commit_message>
Land in kha + optimization with plot
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Interventions/Ecopulpers.xlsx
+++ b/CVX_Kenya/Interventions/Ecopulpers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\CVX_Kenya\Interventions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\Interventions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3BEAA8-1E39-4E9B-A637-1179544EF1FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3FBE34-44C8-4269-90A5-91D0FD364531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="-18225" windowWidth="17280" windowHeight="8970" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -1444,16 +1444,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>-2.8687499999999998E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1500,16 +1500,16 @@
       </c>
       <c r="E3" s="32">
         <f>main!C31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.8259730775000002E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
@@ -1530,15 +1530,15 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1588,16 +1588,16 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
   </sheetData>
@@ -1621,28 +1621,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+    <sheetView zoomScale="113" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>3.375E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>6.7628632500000072E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1788,12 +1788,12 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
@@ -1841,17 +1841,17 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
     <col min="2" max="2" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1910,16 +1910,16 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
@@ -1961,17 +1961,17 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>231</v>
       </c>
@@ -1993,14 +1993,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="56.85546875" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.88671875" customWidth="1"/>
+    <col min="3" max="3" width="47.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -2552,87 +2552,87 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -2646,22 +2646,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="81.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="81.6640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>174</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
         <v>172</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="53"/>
       <c r="B3" s="17" t="s">
         <v>173</v>
@@ -2718,7 +2718,7 @@
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="53"/>
       <c r="B4" s="17" t="s">
         <v>240</v>
@@ -2733,7 +2733,7 @@
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="53"/>
       <c r="B5" s="17" t="s">
         <v>189</v>
@@ -2748,13 +2748,13 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="53"/>
       <c r="B6" s="39" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="40">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24" t="s">
@@ -2765,7 +2765,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="53"/>
       <c r="B7" s="17" t="s">
         <v>191</v>
@@ -2778,7 +2778,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="53"/>
       <c r="B8" s="17" t="s">
         <v>194</v>
@@ -2793,7 +2793,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="53"/>
       <c r="B9" s="17" t="s">
         <v>198</v>
@@ -2808,7 +2808,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="53"/>
       <c r="B10" s="17" t="s">
         <v>201</v>
@@ -2821,7 +2821,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="53"/>
       <c r="B11" s="17" t="s">
         <v>200</v>
@@ -2836,7 +2836,7 @@
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="53"/>
       <c r="B12" s="17" t="s">
         <v>207</v>
@@ -2851,7 +2851,7 @@
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="53"/>
       <c r="B13" s="17" t="s">
         <v>209</v>
@@ -2866,7 +2866,7 @@
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="53"/>
       <c r="B14" s="17" t="s">
         <v>210</v>
@@ -2883,7 +2883,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="53"/>
       <c r="B15" s="17" t="s">
         <v>186</v>
@@ -2896,7 +2896,7 @@
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="53"/>
       <c r="B16" s="17" t="s">
         <v>226</v>
@@ -2911,7 +2911,7 @@
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
         <v>222</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="F17" s="46"/>
       <c r="G17" s="46"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
         <v>180</v>
       </c>
@@ -2941,7 +2941,7 @@
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="51"/>
       <c r="B19" s="16" t="s">
         <v>188</v>
@@ -2956,7 +2956,7 @@
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="51"/>
       <c r="B20" s="16" t="s">
         <v>223</v>
@@ -2971,7 +2971,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="50" t="s">
         <v>181</v>
       </c>
@@ -2989,7 +2989,7 @@
       <c r="F21" s="23"/>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="50"/>
       <c r="B22" s="29" t="s">
         <v>224</v>
@@ -3003,7 +3003,7 @@
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="50"/>
       <c r="B23" s="29" t="s">
         <v>185</v>
@@ -3017,7 +3017,7 @@
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="50"/>
       <c r="B24" s="22" t="s">
         <v>204</v>
@@ -3033,14 +3033,14 @@
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="50"/>
       <c r="B25" s="22" t="s">
         <v>233</v>
       </c>
       <c r="C25" s="31">
         <f>C24*C6*C17</f>
-        <v>0</v>
+        <v>182.59730775000003</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27" t="s">
@@ -3049,7 +3049,7 @@
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="50"/>
       <c r="B26" s="22" t="s">
         <v>206</v>
@@ -3065,7 +3065,7 @@
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="49" t="s">
         <v>182</v>
       </c>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="49"/>
       <c r="B28" s="19" t="s">
         <v>184</v>
@@ -3103,7 +3103,7 @@
       </c>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="49"/>
       <c r="B29" s="19" t="s">
         <v>185</v>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="49"/>
       <c r="B30" s="19" t="s">
         <v>192</v>
@@ -3139,14 +3139,14 @@
       </c>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="49"/>
       <c r="B31" s="19" t="s">
         <v>232</v>
       </c>
       <c r="C31" s="30">
         <f>C25/(10^6)</f>
-        <v>0</v>
+        <v>1.8259730775000002E-4</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="26" t="s">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="49"/>
       <c r="B32" s="19" t="s">
         <v>228</v>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="G32" s="20"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="49"/>
       <c r="B33" s="19" t="s">
         <v>241</v>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="G33" s="20"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="49"/>
       <c r="B34" s="19" t="s">
         <v>193</v>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="G34" s="20"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B37" s="28"/>
     </row>
   </sheetData>

</xml_diff>